<commit_message>
fixed randomness for every experiment
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Download/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jason/GitHub/Research/Traffic_Simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Experiment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Taxi Arrival time</t>
   </si>
@@ -38,14 +36,17 @@
     <t>Estimated arrival time (in second, not include the time for waiting traffic lights)</t>
   </si>
   <si>
-    <t>Difference in arrival time of the called taxi and the first taxi (in minute)</t>
+    <t>Difference in arrival time between the called taxi and the first taxi (in minute)</t>
+  </si>
+  <si>
+    <t>Experiment (500 cars, 20 taxis, initially 80% on major roads)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,6 +58,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -93,30 +110,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,137 +445,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>79.319999999999993</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="12">
+        <f>(MAX(E2:P2) -E2)/60</f>
         <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>41.54</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
+        <f>(MAX(E3:P3) -E3)/60</f>
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>45.83</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="12">
+        <f>(MAX(E4:P4) -E4)/60</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>87.93</v>
       </c>
-      <c r="D5" s="10">
-        <f>(J5-E5)/ 60</f>
+      <c r="D5" s="12">
+        <f>(MAX(E5:P5) -E5)/60</f>
         <v>2.1333333333333333</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>590</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>671</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>681</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>709</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>712</v>
       </c>
       <c r="J5" s="1">
         <v>718</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>55.27</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="12">
+        <f>(MAX(E6:P6) -E6)/60</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>72.25</v>
       </c>
-      <c r="D7" s="10">
-        <f>(G7-E7)/60</f>
+      <c r="D7" s="12">
+        <f>(MAX(E7:P7) -E7)/60</f>
         <v>1.3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>724</v>
       </c>
       <c r="F7">
@@ -532,306 +592,514 @@
         <v>802</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>23.58</v>
       </c>
-      <c r="D8" s="11">
-        <f>(M8-E8)/60</f>
+      <c r="D8" s="13">
+        <f>(MAX(E8:P8) -E8)/60</f>
         <v>8.9666666666666668</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>157</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>432</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>435</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>496</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>511</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>578</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>589</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="3">
         <v>633</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <v>695</v>
       </c>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="N8" s="4"/>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>95.4</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10">
-        <f>(G9-E9)/60</f>
+      <c r="C9" s="6"/>
+      <c r="D9" s="12">
+        <f>(MAX(E9:P9) -E9)/60</f>
         <v>4.8166666666666664</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>372</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>513</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>661</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>32</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10">
-        <f>(MAX(E10:M10) -E10)/60</f>
+      <c r="C10" s="6"/>
+      <c r="D10" s="12">
+        <f>(MAX(E10:P10) -E10)/60</f>
         <v>2.8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>247</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>331</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>415</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>87.67</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10">
-        <f t="shared" ref="D11:D21" si="0">(MAX(E11:M11) -E11)/60</f>
+      <c r="C11" s="6"/>
+      <c r="D11" s="12">
+        <f>(MAX(E11:P11) -E11)/60</f>
         <v>0.96666666666666667</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <v>348</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>406</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>107.16</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10">
-        <f t="shared" si="0"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="12">
+        <f>(MAX(E12:P12) -E12)/60</f>
         <v>8.7166666666666668</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>466</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>926</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>936</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>989</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>89.33</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="12">
-        <f t="shared" si="0"/>
+        <f>(MAX(E13:P13) -E13)/60</f>
         <v>0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>481</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>208.02</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10">
-        <f t="shared" si="0"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="12">
+        <f>(MAX(E14:P14) -E14)/60</f>
         <v>0.36666666666666664</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>732</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>754</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>255.24</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10">
-        <f t="shared" si="0"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
+        <f>(MAX(E15:P15) -E15)/60</f>
         <v>6.4666666666666668</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="6">
         <v>325</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <v>474</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>713</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>71.739999999999995</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10">
-        <f t="shared" si="0"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12">
+        <f>(MAX(E16:P16) -E16)/60</f>
         <v>4.2666666666666666</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="6">
         <v>396</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <v>640</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="6">
         <v>651</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <v>652</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>147.19</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="10">
-        <f t="shared" si="0"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="12">
+        <f>(MAX(E17:P17) -E17)/60</f>
         <v>1.2666666666666666</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>488</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>564</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>146.19</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="10">
-        <f t="shared" si="0"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="12">
+        <f>(MAX(E18:P18) -E18)/60</f>
         <v>6.2166666666666668</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="6">
         <v>338</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="6">
         <v>496</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="6">
         <v>510</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>711</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>124.82</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="12">
-        <f t="shared" si="0"/>
+        <f>(MAX(E19:P19) -E19)/60</f>
         <v>0</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>733</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>181.85</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="12">
-        <f t="shared" si="0"/>
+        <f>(MAX(E20:P20) -E20)/60</f>
         <v>0</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>413</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>106.2</v>
       </c>
       <c r="D21" s="12">
-        <f t="shared" si="0"/>
+        <f>(MAX(E21:P21) -E21)/60</f>
         <v>0</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>596</v>
       </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
+        <v>95.49</v>
+      </c>
+      <c r="D22" s="12">
+        <f>(MAX(E22:P22) -E22)/60</f>
+        <v>6.583333333333333</v>
+      </c>
+      <c r="E22" s="6">
+        <v>218</v>
+      </c>
+      <c r="F22" s="7">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>201.48</v>
+      </c>
+      <c r="D23" s="12">
+        <f>(MAX(E23:P23) -E23)/60</f>
+        <v>8.4333333333333336</v>
+      </c>
+      <c r="E23" s="6">
+        <v>263</v>
+      </c>
+      <c r="F23" s="6">
+        <v>355</v>
+      </c>
+      <c r="G23" s="6">
+        <v>411</v>
+      </c>
+      <c r="H23" s="6">
+        <v>686</v>
+      </c>
+      <c r="I23" s="7">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>118.35</v>
+      </c>
+      <c r="D24" s="12">
+        <f>(MAX(E24:P24) -E24)/60</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>30.86</v>
+      </c>
+      <c r="D25" s="12">
+        <f>(MAX(E25:P25) -E25)/60</f>
+        <v>4.1833333333333336</v>
+      </c>
+      <c r="E25">
+        <v>323</v>
+      </c>
+      <c r="F25">
+        <v>376</v>
+      </c>
+      <c r="G25">
+        <v>545</v>
+      </c>
+      <c r="H25" s="1">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6">
+        <v>129.05000000000001</v>
+      </c>
+      <c r="D26" s="12">
+        <f>(MAX(E26:P26) -E26)/60</f>
+        <v>5.1333333333333337</v>
+      </c>
+      <c r="E26">
+        <v>339</v>
+      </c>
+      <c r="F26">
+        <v>555</v>
+      </c>
+      <c r="G26">
+        <v>637</v>
+      </c>
+      <c r="H26" s="1">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6">
+        <v>139.35</v>
+      </c>
+      <c r="D27" s="12">
+        <f>(MAX(E27:P27) -E27)/60</f>
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="E27">
+        <v>445</v>
+      </c>
+      <c r="F27" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6">
+        <v>110.59</v>
+      </c>
+      <c r="D28" s="12">
+        <f>(MAX(E28:P28) -E28)/60</f>
+        <v>1.4833333333333334</v>
+      </c>
+      <c r="E28">
+        <v>513</v>
+      </c>
+      <c r="F28" s="1">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <v>89.41</v>
+      </c>
+      <c r="D29" s="12">
+        <f>(MAX(E29:P29) -E29)/60</f>
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="E29">
+        <v>439</v>
+      </c>
+      <c r="F29" s="1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
commit before check randomness
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Only update the called taxi" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
   <si>
     <t>Taxi Arrival time</t>
   </si>
@@ -41,12 +42,27 @@
   <si>
     <t>Experiment (500 cars, 20 taxis, initially 80% on major roads)</t>
   </si>
+  <si>
+    <t>Experiment SEED (500 cars, 20 taxis, initially 80% on major roads)</t>
+  </si>
+  <si>
+    <t>update route every 30 second</t>
+  </si>
+  <si>
+    <t>no update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not update route </t>
+  </si>
+  <si>
+    <t>Update route every 30s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +94,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -93,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -139,8 +162,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -150,8 +184,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -180,16 +222,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -200,6 +262,1107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0603864829396325"/>
+          <c:y val="0.0254283318751823"/>
+          <c:w val="0.889613517060367"/>
+          <c:h val="0.575632473024205"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Update route every 30s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$E$30:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$31:$N$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not update route </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$E$30:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$32:$N$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2106283616"/>
+        <c:axId val="2132985648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2106283616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Arrival Order</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132985648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2132985648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2106283616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="1.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1644650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,11 +1657,11 @@
       <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="P1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1093,23 +2256,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="17" customWidth="1"/>
+    <col min="6" max="14" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="144" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>2</v>
@@ -1121,238 +2286,931 @@
       <c r="E1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>54.07</v>
-      </c>
-      <c r="E2" s="17">
-        <v>254</v>
-      </c>
-      <c r="F2">
-        <v>310</v>
-      </c>
-      <c r="G2">
-        <v>329</v>
-      </c>
-      <c r="H2" s="1">
-        <v>329</v>
-      </c>
-      <c r="I2">
-        <v>468</v>
-      </c>
-      <c r="J2">
-        <v>835</v>
-      </c>
-      <c r="K2">
-        <v>1019</v>
-      </c>
-      <c r="L2">
-        <v>1508</v>
-      </c>
-      <c r="M2">
-        <v>2228</v>
-      </c>
-      <c r="N2">
-        <v>2274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>54.07</v>
-      </c>
-      <c r="E3" s="17">
-        <v>254</v>
-      </c>
-      <c r="F3">
-        <v>310</v>
-      </c>
-      <c r="G3">
-        <v>329</v>
-      </c>
-      <c r="H3" s="1">
-        <v>329</v>
-      </c>
-      <c r="I3">
-        <v>468</v>
-      </c>
-      <c r="J3">
-        <v>835</v>
-      </c>
-      <c r="K3">
-        <v>1019</v>
-      </c>
-      <c r="L3">
-        <v>1508</v>
-      </c>
-      <c r="M3">
-        <v>2228</v>
-      </c>
-      <c r="N3">
-        <v>2274</v>
+        <v>114.53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="21">
+        <v>703</v>
+      </c>
+      <c r="F2" s="6">
+        <v>952</v>
+      </c>
+      <c r="G2" s="6">
+        <v>952</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1095</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1105</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1472</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1702</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2103</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2258</v>
+      </c>
+      <c r="N2" s="6">
+        <v>2714</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>114.53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="22">
+        <v>584</v>
+      </c>
+      <c r="F3" s="4">
+        <v>698</v>
+      </c>
+      <c r="G3" s="5">
+        <v>766</v>
+      </c>
+      <c r="H3" s="4">
+        <v>776</v>
+      </c>
+      <c r="I3" s="4">
+        <v>958</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1021</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1317</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1337</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1490</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1702</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>54.07</v>
-      </c>
-      <c r="E4" s="17">
-        <v>254</v>
-      </c>
-      <c r="F4">
-        <v>310</v>
-      </c>
-      <c r="G4">
-        <v>329</v>
-      </c>
-      <c r="H4" s="1">
-        <v>329</v>
-      </c>
-      <c r="I4">
-        <v>468</v>
-      </c>
-      <c r="J4">
-        <v>835</v>
-      </c>
-      <c r="K4">
-        <v>1019</v>
-      </c>
-      <c r="L4">
-        <v>1508</v>
-      </c>
-      <c r="M4">
-        <v>2228</v>
-      </c>
-      <c r="N4">
-        <v>2274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>54.07</v>
-      </c>
-      <c r="E5" s="17">
-        <v>254</v>
-      </c>
-      <c r="F5">
-        <v>310</v>
-      </c>
-      <c r="G5">
-        <v>329</v>
-      </c>
-      <c r="H5" s="1">
-        <v>329</v>
-      </c>
-      <c r="I5">
-        <v>468</v>
-      </c>
-      <c r="J5">
-        <v>835</v>
-      </c>
-      <c r="K5">
-        <v>1019</v>
-      </c>
-      <c r="L5">
-        <v>1508</v>
-      </c>
-      <c r="M5">
-        <v>2228</v>
-      </c>
-      <c r="N5">
-        <v>2274</v>
+        <v>136.13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="21">
+        <v>405</v>
+      </c>
+      <c r="F4" s="6">
+        <v>830</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1074</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1139</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1335</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1586</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1651</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1756</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1904</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>133.88</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="4">
+        <v>395</v>
+      </c>
+      <c r="F5" s="5">
+        <v>486</v>
+      </c>
+      <c r="G5" s="4">
+        <v>829</v>
+      </c>
+      <c r="H5" s="4">
+        <v>912</v>
+      </c>
+      <c r="I5" s="4">
+        <v>997</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1075</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1141</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1249</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1418</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1482</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>127.11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="21">
+        <v>497</v>
+      </c>
+      <c r="F6" s="7">
+        <v>746</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1121</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1386</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1582</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1655</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1832</v>
+      </c>
+      <c r="L6" s="6">
+        <v>2366</v>
+      </c>
+      <c r="M6" s="6">
+        <v>2451</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>127.11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="22">
+        <v>408</v>
+      </c>
+      <c r="F7" s="4">
+        <v>494</v>
+      </c>
+      <c r="G7" s="5">
+        <v>586</v>
+      </c>
+      <c r="H7" s="4">
+        <v>883</v>
+      </c>
+      <c r="I7" s="4">
+        <v>912</v>
+      </c>
+      <c r="J7" s="4">
+        <v>951</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1119</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1310</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1365</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>134.86000000000001</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="21">
+        <v>518</v>
+      </c>
+      <c r="F8" s="6">
+        <v>834</v>
+      </c>
+      <c r="G8" s="6">
+        <v>846</v>
+      </c>
+      <c r="H8" s="6">
+        <v>865</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1090</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1203</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1217</v>
+      </c>
+      <c r="L8" s="6">
+        <v>2274</v>
+      </c>
+      <c r="M8" s="6">
+        <v>2289</v>
+      </c>
+      <c r="N8" s="6">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3">
+        <v>191.37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="20">
+        <v>606</v>
+      </c>
+      <c r="F9" s="4">
+        <v>606</v>
+      </c>
+      <c r="G9" s="4">
+        <v>670</v>
+      </c>
+      <c r="H9" s="4">
+        <v>910</v>
+      </c>
+      <c r="I9" s="4">
+        <v>922</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1022</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1096</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1182</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1292</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>54.07</v>
-      </c>
-      <c r="E6" s="17">
-        <v>254</v>
-      </c>
-      <c r="F6">
-        <v>310</v>
-      </c>
-      <c r="G6">
-        <v>329</v>
-      </c>
-      <c r="H6" s="1">
-        <v>329</v>
-      </c>
-      <c r="I6">
-        <v>468</v>
-      </c>
-      <c r="J6">
-        <v>835</v>
-      </c>
-      <c r="K6">
-        <v>1019</v>
-      </c>
-      <c r="L6">
-        <v>1508</v>
-      </c>
-      <c r="M6">
-        <v>2228</v>
-      </c>
-      <c r="N6">
-        <v>2274</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B10" s="6">
+        <v>117.13</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>54.07</v>
-      </c>
-      <c r="E7" s="17">
-        <v>254</v>
-      </c>
-      <c r="F7">
-        <v>310</v>
-      </c>
-      <c r="G7">
-        <v>329</v>
-      </c>
-      <c r="H7" s="1">
-        <v>329</v>
-      </c>
-      <c r="I7">
-        <v>468</v>
-      </c>
-      <c r="J7">
-        <v>835</v>
-      </c>
-      <c r="K7">
-        <v>1019</v>
-      </c>
-      <c r="L7">
-        <v>1508</v>
-      </c>
-      <c r="M7">
-        <v>2228</v>
-      </c>
-      <c r="N7">
-        <v>2274</v>
+      <c r="E10" s="21">
+        <v>517</v>
+      </c>
+      <c r="F10" s="6">
+        <v>770</v>
+      </c>
+      <c r="G10" s="6">
+        <v>850</v>
+      </c>
+      <c r="H10" s="7">
+        <v>947</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1214</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1400</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1897</v>
+      </c>
+      <c r="L10" s="6">
+        <v>2264</v>
+      </c>
+      <c r="M10" s="6">
+        <v>2326</v>
+      </c>
+      <c r="N10" s="6">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <v>117.13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="22">
+        <v>680</v>
+      </c>
+      <c r="F11" s="4">
+        <v>680</v>
+      </c>
+      <c r="G11" s="4">
+        <v>680</v>
+      </c>
+      <c r="H11" s="4">
+        <v>765</v>
+      </c>
+      <c r="I11" s="5">
+        <v>838</v>
+      </c>
+      <c r="J11" s="4">
+        <v>950</v>
+      </c>
+      <c r="K11" s="4">
+        <v>964</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1215</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1306</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6">
+        <v>210.41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="21">
+        <v>962</v>
+      </c>
+      <c r="F12" s="6">
+        <v>972</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1220</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1282</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1458</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1479</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1494</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1564</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1718</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>210.96</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="22">
+        <v>336</v>
+      </c>
+      <c r="F13" s="4">
+        <v>614</v>
+      </c>
+      <c r="G13" s="4">
+        <v>937</v>
+      </c>
+      <c r="H13" s="4">
+        <v>948</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1113</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1123</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1219</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1371</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1380</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6">
+        <v>124.98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="19">
+        <v>920</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1011</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1097</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1154</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1266</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1866</v>
+      </c>
+      <c r="K14" s="6">
+        <v>2106</v>
+      </c>
+      <c r="L14" s="6">
+        <v>2120</v>
+      </c>
+      <c r="M14" s="6">
+        <v>2177</v>
+      </c>
+      <c r="N14" s="6">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="20">
+        <v>716</v>
+      </c>
+      <c r="F15" s="4">
+        <v>724</v>
+      </c>
+      <c r="G15" s="4">
+        <v>738</v>
+      </c>
+      <c r="H15" s="3">
+        <v>738</v>
+      </c>
+      <c r="I15" s="4">
+        <v>821</v>
+      </c>
+      <c r="J15" s="4">
+        <v>927</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1096</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1196</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1607</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6">
+        <v>95.83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="21">
+        <v>507</v>
+      </c>
+      <c r="F16" s="6">
+        <v>573</v>
+      </c>
+      <c r="G16" s="7">
+        <v>647</v>
+      </c>
+      <c r="H16" s="6">
+        <v>739</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1039</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1219</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1536</v>
+      </c>
+      <c r="L16" s="6">
+        <v>1593</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1770</v>
+      </c>
+      <c r="N16" s="6">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>95.83</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="22">
+        <v>489</v>
+      </c>
+      <c r="F17" s="5">
+        <v>665</v>
+      </c>
+      <c r="G17" s="4">
+        <v>665</v>
+      </c>
+      <c r="H17" s="4">
+        <v>666</v>
+      </c>
+      <c r="I17" s="4">
+        <v>668</v>
+      </c>
+      <c r="J17" s="4">
+        <v>823</v>
+      </c>
+      <c r="K17" s="4">
+        <v>990</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1121</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1639</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6">
+        <v>39.64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="19">
+        <v>552</v>
+      </c>
+      <c r="F18" s="6">
+        <v>985</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1046</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1589</v>
+      </c>
+      <c r="I18" s="6">
+        <v>1646</v>
+      </c>
+      <c r="J18" s="6">
+        <v>2023</v>
+      </c>
+      <c r="K18" s="6">
+        <v>2195</v>
+      </c>
+      <c r="L18" s="6">
+        <v>2430</v>
+      </c>
+      <c r="M18" s="6">
+        <v>2626</v>
+      </c>
+      <c r="N18" s="6">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6">
+        <v>39.64</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="20">
+        <v>527</v>
+      </c>
+      <c r="F19" s="4">
+        <v>892</v>
+      </c>
+      <c r="G19" s="4">
+        <v>892</v>
+      </c>
+      <c r="H19" s="4">
+        <v>906</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1136</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1420</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1478</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1504</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1589</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6">
+        <v>65.83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="21">
+        <v>156</v>
+      </c>
+      <c r="F20" s="7">
+        <v>421</v>
+      </c>
+      <c r="G20" s="6">
+        <v>434</v>
+      </c>
+      <c r="H20" s="6">
+        <v>509</v>
+      </c>
+      <c r="I20" s="6">
+        <v>576</v>
+      </c>
+      <c r="J20" s="6">
+        <v>763</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1665</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1825</v>
+      </c>
+      <c r="M20" s="6">
+        <v>1835</v>
+      </c>
+      <c r="N20" s="6">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="22">
+        <v>216</v>
+      </c>
+      <c r="F21" s="4">
+        <v>533</v>
+      </c>
+      <c r="G21" s="5">
+        <v>581</v>
+      </c>
+      <c r="H21" s="4">
+        <v>704</v>
+      </c>
+      <c r="I21" s="4">
+        <v>704</v>
+      </c>
+      <c r="J21" s="4">
+        <v>735</v>
+      </c>
+      <c r="K21" s="4">
+        <v>810</v>
+      </c>
+      <c r="L21" s="4">
+        <v>896</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1089</v>
+      </c>
+      <c r="N21" s="4">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E30" s="23">
+        <v>1</v>
+      </c>
+      <c r="F30" s="24">
+        <v>2</v>
+      </c>
+      <c r="G30" s="24">
+        <v>3</v>
+      </c>
+      <c r="H30" s="24">
+        <v>4</v>
+      </c>
+      <c r="I30" s="24">
+        <v>5</v>
+      </c>
+      <c r="J30" s="24">
+        <v>6</v>
+      </c>
+      <c r="K30" s="24">
+        <v>7</v>
+      </c>
+      <c r="L30" s="24">
+        <v>8</v>
+      </c>
+      <c r="M30" s="24">
+        <v>9</v>
+      </c>
+      <c r="N30" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D31" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="26">
+        <v>2</v>
+      </c>
+      <c r="F31" s="27">
+        <v>2</v>
+      </c>
+      <c r="G31" s="27">
+        <v>1</v>
+      </c>
+      <c r="H31" s="27">
+        <v>3</v>
+      </c>
+      <c r="I31" s="27">
+        <v>0</v>
+      </c>
+      <c r="J31" s="27">
+        <v>1</v>
+      </c>
+      <c r="K31" s="27">
+        <v>0</v>
+      </c>
+      <c r="L31" s="27">
+        <v>1</v>
+      </c>
+      <c r="M31" s="27">
+        <v>0</v>
+      </c>
+      <c r="N31" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D32" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="26">
+        <v>3</v>
+      </c>
+      <c r="F32" s="27">
+        <v>2</v>
+      </c>
+      <c r="G32" s="27">
+        <v>3</v>
+      </c>
+      <c r="H32" s="27">
+        <v>0</v>
+      </c>
+      <c r="I32" s="27">
+        <v>1</v>
+      </c>
+      <c r="J32" s="27">
+        <v>0</v>
+      </c>
+      <c r="K32" s="27">
+        <v>0</v>
+      </c>
+      <c r="L32" s="27">
+        <v>1</v>
+      </c>
+      <c r="M32" s="27">
+        <v>0</v>
+      </c>
+      <c r="N32" s="27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1361,5 +3219,437 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="128" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>